<commit_message>
Update all drawing python and data for camera ready version
</commit_message>
<xml_diff>
--- a/Benchmark/Benchmark.xlsx
+++ b/Benchmark/Benchmark.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linli\Desktop\Evaluation\Benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LabDOC\draw\EvaluationScript\Benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7929717-B9D8-4FB1-A7BD-76FDCBEFE681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2CB3B7-663F-45C4-9E0B-1F4962B82366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="-105" windowWidth="28995" windowHeight="15675" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3DMark_External" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -38,9 +29,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="21">
-  <si>
-    <t>VMWare</t>
-  </si>
   <si>
     <t>Native PC</t>
   </si>
@@ -131,12 +119,38 @@
     <t>T-Rex Offscreen</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>VM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>are</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,6 +170,13 @@
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -507,53 +528,53 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.19921875" customWidth="1"/>
-    <col min="7" max="7" width="17.796875" customWidth="1"/>
-    <col min="1023" max="1023" width="9.1328125" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="7.625" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="1023" max="1023" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>21236</v>
@@ -576,7 +597,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>67973</v>
@@ -602,7 +623,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>320.5</v>
@@ -628,7 +649,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>274.2</v>
@@ -654,7 +675,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>6234</v>
@@ -677,7 +698,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>155</v>
@@ -700,7 +721,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>64.599999999999994</v>
@@ -723,7 +744,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>30.9</v>
@@ -746,7 +767,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>21120</v>
@@ -769,7 +790,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>65203</v>
@@ -795,7 +816,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>327.39999999999998</v>
@@ -821,7 +842,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>249.9</v>
@@ -847,7 +868,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>6274</v>
@@ -870,7 +891,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>157</v>
@@ -893,7 +914,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>64.900000000000006</v>
@@ -916,7 +937,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>31</v>
@@ -939,7 +960,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>21089</v>
@@ -962,7 +983,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21">
         <v>66500</v>
@@ -988,7 +1009,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>330.7</v>
@@ -1014,7 +1035,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>256.89999999999998</v>
@@ -1040,7 +1061,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>6221</v>
@@ -1063,7 +1084,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>150.80000000000001</v>
@@ -1086,7 +1107,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>65.5</v>
@@ -1109,7 +1130,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>30.8</v>
@@ -1132,7 +1153,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29">
         <v>21079</v>
@@ -1155,7 +1176,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30">
         <v>64606</v>
@@ -1181,7 +1202,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>320.3</v>
@@ -1207,7 +1228,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32">
         <v>250.1</v>
@@ -1233,7 +1254,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33">
         <v>6277</v>
@@ -1256,7 +1277,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34">
         <v>153.9</v>
@@ -1279,7 +1300,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35">
         <v>65.2</v>
@@ -1302,7 +1323,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>31.2</v>
@@ -1325,7 +1346,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38">
         <v>20747</v>
@@ -1348,7 +1369,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39">
         <v>62647</v>
@@ -1374,7 +1395,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40">
         <v>302.3</v>
@@ -1400,7 +1421,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41">
         <v>247.9</v>
@@ -1426,7 +1447,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42">
         <v>6210</v>
@@ -1449,7 +1470,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43">
         <v>153.19999999999999</v>
@@ -1472,7 +1493,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44">
         <v>65.7</v>
@@ -1495,7 +1516,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45">
         <v>30.4</v>
@@ -1518,7 +1539,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47">
         <f t="shared" ref="B47:E54" si="0">AVERAGE(B38,B29,B20,B11,B2)</f>
@@ -1543,7 +1564,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
@@ -1568,7 +1589,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
@@ -1593,7 +1614,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
@@ -1618,7 +1639,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
@@ -1643,7 +1664,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
@@ -1668,7 +1689,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
@@ -1693,7 +1714,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
@@ -1727,54 +1748,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.796875" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>3481</v>
@@ -1797,7 +1818,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>6132</v>
@@ -1823,7 +1844,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>32.6</v>
@@ -1849,7 +1870,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>22.6</v>
@@ -1875,7 +1896,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1385</v>
@@ -1898,7 +1919,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>30.8</v>
@@ -1921,7 +1942,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>13.4</v>
@@ -1944,7 +1965,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>7.5</v>
@@ -1967,7 +1988,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>3445</v>
@@ -1990,7 +2011,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>6092</v>
@@ -2016,7 +2037,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>32</v>
@@ -2042,7 +2063,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>22.6</v>
@@ -2068,7 +2089,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>1367</v>
@@ -2091,7 +2112,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>32.700000000000003</v>
@@ -2114,7 +2135,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>14.3</v>
@@ -2137,7 +2158,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>6.8</v>
@@ -2160,7 +2181,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>3451</v>
@@ -2183,7 +2204,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21">
         <v>6102</v>
@@ -2209,7 +2230,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>32</v>
@@ -2235,7 +2256,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>22.7</v>
@@ -2261,7 +2282,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>1369</v>
@@ -2284,7 +2305,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>32</v>
@@ -2307,7 +2328,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>14.3</v>
@@ -2330,7 +2351,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>6.9</v>
@@ -2353,7 +2374,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29">
         <v>3480</v>
@@ -2376,7 +2397,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30">
         <v>6168</v>
@@ -2402,7 +2423,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>32.200000000000003</v>
@@ -2428,7 +2449,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32">
         <v>23</v>
@@ -2454,7 +2475,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33">
         <v>1378</v>
@@ -2477,7 +2498,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34">
         <v>32.200000000000003</v>
@@ -2500,7 +2521,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35">
         <v>14.5</v>
@@ -2523,7 +2544,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>6.9</v>
@@ -2546,7 +2567,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38">
         <v>3464</v>
@@ -2569,7 +2590,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39">
         <v>6142</v>
@@ -2595,7 +2616,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40">
         <v>31.9</v>
@@ -2621,7 +2642,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41">
         <v>23</v>
@@ -2647,7 +2668,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42">
         <v>1371</v>
@@ -2670,7 +2691,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43">
         <v>32.4</v>
@@ -2693,7 +2714,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44">
         <v>14.2</v>
@@ -2716,7 +2737,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45">
         <v>6.9</v>
@@ -2739,7 +2760,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47">
         <f t="shared" ref="B47:C50" si="0">AVERAGE(B38,B29,B20,B11,B2)</f>
@@ -2764,7 +2785,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
@@ -2793,7 +2814,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
@@ -2822,7 +2843,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
@@ -2851,7 +2872,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51">
         <f>AVERAGE(B42,B33,B24,B15,B6)</f>
@@ -2876,7 +2897,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B52">
         <f>AVERAGE(B43,B34,B25,B16,B7)</f>
@@ -2901,7 +2922,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53">
         <f>AVERAGE(B44,B35,B26,B17,B8)</f>
@@ -2926,7 +2947,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54">
         <f>AVERAGE(B45,B36,B27,B18,B9)</f>
@@ -2961,53 +2982,53 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A30"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="13.46484375" customWidth="1"/>
-    <col min="3" max="3" width="7.86328125" customWidth="1"/>
-    <col min="4" max="4" width="11.46484375" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.86328125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="7.875" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.125" customWidth="1"/>
+    <col min="6" max="6" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="9.875" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>60</v>
@@ -3027,7 +3048,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>226</v>
@@ -3053,7 +3074,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>60</v>
@@ -3073,7 +3094,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>828</v>
@@ -3099,7 +3120,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>60</v>
@@ -3122,7 +3143,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>204</v>
@@ -3148,7 +3169,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>61</v>
@@ -3171,7 +3192,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>810</v>
@@ -3197,7 +3218,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>61</v>
@@ -3217,7 +3238,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>219</v>
@@ -3243,7 +3264,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>60</v>
@@ -3263,7 +3284,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>811</v>
@@ -3289,7 +3310,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>62</v>
@@ -3309,7 +3330,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>233</v>
@@ -3335,7 +3356,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>60</v>
@@ -3355,7 +3376,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>882</v>
@@ -3381,7 +3402,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>60</v>
@@ -3401,7 +3422,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23">
         <v>208</v>
@@ -3427,7 +3448,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>60</v>
@@ -3447,7 +3468,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>859</v>
@@ -3473,7 +3494,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27">
         <f>AVERAGE(C2,C7,C12,C17,C22)</f>
@@ -3502,7 +3523,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <f>AVERAGE(C3,C8,C13,C18,C23)</f>
@@ -3531,7 +3552,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29">
         <f>AVERAGE(C4,C9,C14,C19,C24)</f>
@@ -3560,7 +3581,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <f>AVERAGE(C5,C10,C15,C20,C25)</f>
@@ -3598,59 +3619,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.796875" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="13.625" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>31</v>
@@ -3676,12 +3697,12 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3707,12 +3728,12 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>32</v>
@@ -3738,12 +3759,12 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>103</v>
@@ -3769,12 +3790,12 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>32</v>
@@ -3800,12 +3821,12 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>102</v>
@@ -3831,12 +3852,12 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>32</v>
@@ -3862,12 +3883,12 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>103</v>
@@ -3893,12 +3914,12 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23">
         <v>32</v>
@@ -3924,12 +3945,12 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>104</v>
@@ -3955,12 +3976,12 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <f>AVERAGE(C3,C8,C13,C18,C23)</f>
@@ -3985,12 +4006,12 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <f>AVERAGE(C5,C10,C15,C20,C25)</f>

</xml_diff>